<commit_message>
Fixed misconception of TTD:PDSpec relationship. Already satisfied by Equipment:PDSpec relationship
</commit_message>
<xml_diff>
--- a/Relationships/Table Relations Matrix.xlsx
+++ b/Relationships/Table Relations Matrix.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\csc410-labs-jz\Relationships\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0DF0D6-8483-4F66-BE42-3C5B202B42F6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -91,21 +100,29 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-    </font>
-    <font/>
-    <font>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
@@ -115,7 +132,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -131,68 +148,364 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="53.57"/>
-    <col customWidth="1" min="3" max="3" width="23.57"/>
-    <col customWidth="1" min="9" max="9" width="17.14"/>
-    <col customWidth="1" min="10" max="10" width="18.0"/>
-    <col customWidth="1" min="17" max="17" width="20.86"/>
-    <col customWidth="1" min="18" max="18" width="23.57"/>
-    <col customWidth="1" min="19" max="19" width="26.0"/>
-    <col customWidth="1" min="21" max="21" width="17.0"/>
-    <col customWidth="1" min="22" max="22" width="16.86"/>
+    <col min="1" max="1" width="53.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="17" max="17" width="20.88671875" customWidth="1"/>
+    <col min="18" max="18" width="23.5546875" customWidth="1"/>
+    <col min="19" max="19" width="26" customWidth="1"/>
+    <col min="21" max="21" width="17" customWidth="1"/>
+    <col min="22" max="22" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -262,7 +575,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -330,7 +643,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -398,7 +711,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -466,7 +779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -534,7 +847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -602,7 +915,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -670,7 +983,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -738,7 +1051,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -793,8 +1106,8 @@
       <c r="R9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="S9" s="5" t="s">
-        <v>22</v>
+      <c r="S9" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>21</v>
@@ -806,7 +1119,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -874,7 +1187,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -942,7 +1255,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1008,7 +1321,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1076,7 +1389,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1144,7 +1457,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1212,7 +1525,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1280,7 +1593,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:22" ht="15.75" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1348,7 +1661,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:22" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1416,7 +1729,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:22" ht="13.2">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1441,8 +1754,8 @@
       <c r="H19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>23</v>
+      <c r="I19" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>21</v>
@@ -1484,7 +1797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:22" ht="13.2">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1552,7 +1865,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:22" ht="13.2">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1620,7 +1933,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:22" ht="13.2">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1689,6 +2002,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created AssemblyParts table, removed unneeded specs (kept in non-use folder). Removed unneeded relationships from matrix.
</commit_message>
<xml_diff>
--- a/Relationships/Table Relations Matrix.xlsx
+++ b/Relationships/Table Relations Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\csc410-labs-jz\Relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0DF0D6-8483-4F66-BE42-3C5B202B42F6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8279C3-4C87-4F02-AE63-2256DDF41BB5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="26">
   <si>
     <t>Equipment</t>
   </si>
@@ -95,13 +95,16 @@
   </si>
   <si>
     <t>Blow Down Devices</t>
+  </si>
+  <si>
+    <t>Assembly Parts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -125,6 +128,24 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -159,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -169,6 +190,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +514,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z22"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -540,7 +568,7 @@
       <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -570,7 +598,9 @@
       <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1"/>
+      <c r="W1" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
@@ -642,6 +672,9 @@
       <c r="V2" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="W2" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -710,6 +743,9 @@
       <c r="V3" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="W3" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -778,6 +814,9 @@
       <c r="V4" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="W4" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
@@ -846,6 +885,9 @@
       <c r="V5" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="W5" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
@@ -914,6 +956,9 @@
       <c r="V6" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="W6" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -982,6 +1027,9 @@
       <c r="V7" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="W7" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
@@ -1008,11 +1056,11 @@
       <c r="H8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>22</v>
+      <c r="I8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>21</v>
@@ -1048,6 +1096,9 @@
         <v>21</v>
       </c>
       <c r="V8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W8" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1073,8 +1124,8 @@
       <c r="G9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>22</v>
+      <c r="H9" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>21</v>
@@ -1088,8 +1139,8 @@
       <c r="L9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="5" t="s">
-        <v>23</v>
+      <c r="M9" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>21</v>
@@ -1116,6 +1167,9 @@
         <v>22</v>
       </c>
       <c r="V9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W9" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1141,8 +1195,8 @@
       <c r="G10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>22</v>
+      <c r="H10" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>21</v>
@@ -1162,8 +1216,8 @@
       <c r="N10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="5" t="s">
-        <v>23</v>
+      <c r="O10" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>21</v>
@@ -1184,6 +1238,9 @@
         <v>21</v>
       </c>
       <c r="V10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W10" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1254,6 +1311,9 @@
       <c r="V11" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="W11" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
@@ -1295,8 +1355,8 @@
       <c r="M12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="5" t="s">
-        <v>23</v>
+      <c r="N12" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>21</v>
@@ -1318,6 +1378,9 @@
         <v>21</v>
       </c>
       <c r="V12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W12" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1346,8 +1409,8 @@
       <c r="H13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>23</v>
+      <c r="I13" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>21</v>
@@ -1386,6 +1449,9 @@
         <v>21</v>
       </c>
       <c r="V13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W13" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1414,8 +1480,8 @@
       <c r="H14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>23</v>
+      <c r="I14" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>21</v>
@@ -1423,11 +1489,11 @@
       <c r="K14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>23</v>
+      <c r="L14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>21</v>
@@ -1454,6 +1520,9 @@
         <v>21</v>
       </c>
       <c r="V14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W14" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1485,8 +1554,8 @@
       <c r="I15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="5" t="s">
-        <v>22</v>
+      <c r="J15" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>21</v>
@@ -1522,6 +1591,9 @@
         <v>21</v>
       </c>
       <c r="V15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W15" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1550,11 +1622,11 @@
       <c r="H16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>23</v>
+      <c r="I16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>21</v>
@@ -1592,8 +1664,11 @@
       <c r="V16" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" ht="15.75" customHeight="1">
+      <c r="W16" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="15.75" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1660,8 +1735,11 @@
       <c r="V17" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" ht="15.75" customHeight="1">
+      <c r="W17" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1728,8 +1806,11 @@
       <c r="V18" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" ht="13.2">
+      <c r="W18" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="13.2">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1796,8 +1877,11 @@
       <c r="V19" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" ht="13.2">
+      <c r="W19" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="13.2">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1864,8 +1948,11 @@
       <c r="V20" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" ht="13.2">
+      <c r="W20" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="13.2">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1932,8 +2019,11 @@
       <c r="V21" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" ht="13.2">
+      <c r="W21" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="13.2">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1964,8 +2054,8 @@
       <c r="J22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K22" s="5" t="s">
-        <v>23</v>
+      <c r="K22" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>21</v>
@@ -1998,10 +2088,85 @@
         <v>21</v>
       </c>
       <c r="V22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W22" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="15.75" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="R23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="S23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="U23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="V23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="W23" s="11" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added table to handle multiple BDOnTimes (as requested by Paul). Removed redundant fields/fields handled by other tables.
</commit_message>
<xml_diff>
--- a/Relationships/Table Relations Matrix.xlsx
+++ b/Relationships/Table Relations Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\csc410-labs-jz\Relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8279C3-4C87-4F02-AE63-2256DDF41BB5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82003A13-BE96-40E5-A49D-D03D7299C449}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="27">
   <si>
     <t>Equipment</t>
   </si>
@@ -97,14 +97,17 @@
     <t>Blow Down Devices</t>
   </si>
   <si>
-    <t>Assembly Parts</t>
+    <t>Blowdown Specification On Times</t>
+  </si>
+  <si>
+    <t>BlowdownSpecification On Times</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -128,13 +131,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -180,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -191,12 +187,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +506,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -531,9 +523,10 @@
     <col min="19" max="19" width="26" customWidth="1"/>
     <col min="21" max="21" width="17" customWidth="1"/>
     <col min="22" max="22" width="16.88671875" customWidth="1"/>
+    <col min="23" max="23" width="30.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1">
+    <row r="1" spans="1:25" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -568,7 +561,7 @@
       <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -598,19 +591,18 @@
       <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="12" t="s">
-        <v>25</v>
+      <c r="W1" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+    </row>
+    <row r="2" spans="1:25" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
+      <c r="B2" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>22</v>
@@ -673,10 +665,10 @@
         <v>23</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -743,11 +735,11 @@
       <c r="V3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W3" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W3" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -769,7 +761,7 @@
       <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -818,7 +810,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
+    <row r="5" spans="1:25" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -885,11 +877,11 @@
       <c r="V5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W5" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -956,11 +948,11 @@
       <c r="V6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W6" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W6" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1027,11 +1019,11 @@
       <c r="V7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W7" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W7" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1056,10 +1048,10 @@
       <c r="H8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>21</v>
       </c>
       <c r="K8" s="3" t="s">
@@ -1098,11 +1090,11 @@
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W8" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W8" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +1131,7 @@
       <c r="L9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="13" t="s">
+      <c r="M9" s="10" t="s">
         <v>21</v>
       </c>
       <c r="N9" s="3" t="s">
@@ -1169,11 +1161,11 @@
       <c r="V9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W9" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W9" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1216,7 +1208,7 @@
       <c r="N10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="13" t="s">
+      <c r="O10" s="10" t="s">
         <v>21</v>
       </c>
       <c r="P10" s="3" t="s">
@@ -1240,11 +1232,11 @@
       <c r="V10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W10" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W10" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1311,11 +1303,11 @@
       <c r="V11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="W11" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W11" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1355,7 +1347,7 @@
       <c r="M12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="13" t="s">
+      <c r="N12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="O12" s="3" t="s">
@@ -1380,11 +1372,11 @@
       <c r="V12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W12" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W12" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1409,7 +1401,7 @@
       <c r="H13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J13" s="3" t="s">
@@ -1451,11 +1443,11 @@
       <c r="V13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W13" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W13" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1480,7 +1472,7 @@
       <c r="H14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J14" s="3" t="s">
@@ -1489,10 +1481,10 @@
       <c r="K14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="13" t="s">
+      <c r="L14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="10" t="s">
         <v>21</v>
       </c>
       <c r="N14" s="3" t="s">
@@ -1522,11 +1514,11 @@
       <c r="V14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W14" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W14" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1554,7 +1546,7 @@
       <c r="I15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="10" t="s">
         <v>21</v>
       </c>
       <c r="K15" s="3" t="s">
@@ -1593,11 +1585,11 @@
       <c r="V15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W15" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+      <c r="W15" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="15.75" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1622,10 +1614,10 @@
       <c r="H16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="13" t="s">
+      <c r="I16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="10" t="s">
         <v>21</v>
       </c>
       <c r="K16" s="3" t="s">
@@ -1664,7 +1656,7 @@
       <c r="V16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W16" s="11" t="s">
+      <c r="W16" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1735,7 +1727,7 @@
       <c r="V17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W17" s="11" t="s">
+      <c r="W17" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1806,8 +1798,8 @@
       <c r="V18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W18" s="11" t="s">
-        <v>21</v>
+      <c r="W18" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="13.2">
@@ -1877,7 +1869,7 @@
       <c r="V19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W19" s="11" t="s">
+      <c r="W19" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1948,7 +1940,7 @@
       <c r="V20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W20" s="11" t="s">
+      <c r="W20" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2019,7 +2011,7 @@
       <c r="V21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W21" s="11" t="s">
+      <c r="W21" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2054,7 +2046,7 @@
       <c r="J22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="K22" s="10" t="s">
         <v>21</v>
       </c>
       <c r="L22" s="3" t="s">
@@ -2090,78 +2082,78 @@
       <c r="V22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W22" s="11" t="s">
+      <c r="W22" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="11" t="s">
+      <c r="B23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="P23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="R23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="S23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="U23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="V23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="W23" s="11" t="s">
+      <c r="I23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="U23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="W23" s="9" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change facilities to plants
</commit_message>
<xml_diff>
--- a/Relationships/Table Relations Matrix.xlsx
+++ b/Relationships/Table Relations Matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\csc410-labs-jz\Relationships\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Google Drive\School\Centre College\2018-2019\Semester 1\CSC 410 - Database Systems\Project\csc410-labs-jz\Relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90D211B-2F4D-496E-B281-F6020CA4455D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FCD111-5C67-41D5-B75C-6431455CC53B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <t>Clients</t>
   </si>
   <si>
-    <t>Facilities</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>Cal Or Sets</t>
+  </si>
+  <si>
+    <t>Plants</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -542,55 +542,55 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
@@ -600,64 +600,64 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="O2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="R2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U2" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1">
@@ -665,64 +665,64 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1">
@@ -730,1167 +730,1167 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="S7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="T7" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="P8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U9" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U10" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U11" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U13" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U14" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="I15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="O15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U15" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="15.75" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U16" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="S16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U16" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="13.2">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U17" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="13.2">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U18" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="13.2">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="13.2">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U20" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>